<commit_message>
Atualizado por script em 07-01-2024 14:45
</commit_message>
<xml_diff>
--- a/2023/cambodia_cpl_2023-2024.xlsx
+++ b/2023/cambodia_cpl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V78"/>
+  <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Visakha</t>
+          <t>Svay Rieng</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,63 +3893,63 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Angkor Tiger</t>
+          <t>Kirivong Sok Sen Chey</t>
         </is>
       </c>
       <c r="I38" t="n">
         <v>1</v>
       </c>
       <c r="J38" t="n">
-        <v>1.15</v>
+        <v>1.11</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>21/10/2023 00:43</t>
+          <t>21/10/2023 00:13</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>1.19</v>
+        <v>1.25</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>22/10/2023 12:45</t>
+          <t>22/10/2023 12:44</t>
         </is>
       </c>
       <c r="N38" t="n">
-        <v>6.29</v>
+        <v>7</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>21/10/2023 00:43</t>
+          <t>21/10/2023 00:13</t>
         </is>
       </c>
       <c r="P38" t="n">
-        <v>6.51</v>
+        <v>5.69</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>22/10/2023 12:45</t>
+          <t>22/10/2023 12:51</t>
         </is>
       </c>
       <c r="R38" t="n">
-        <v>8.19</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>21/10/2023 00:43</t>
+          <t>21/10/2023 00:13</t>
         </is>
       </c>
       <c r="T38" t="n">
-        <v>8.699999999999999</v>
+        <v>7.79</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>22/10/2023 12:45</t>
+          <t>22/10/2023 12:46</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/cambodia/cpl/visakha-angkor-tiger/8YkmqVgG/</t>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/svay-rieng-kirivong-sok-sen-chey/vaoqpBvA/</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Svay Rieng</t>
+          <t>Visakha</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -3985,63 +3985,63 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Kirivong Sok Sen Chey</t>
+          <t>Angkor Tiger</t>
         </is>
       </c>
       <c r="I39" t="n">
         <v>1</v>
       </c>
       <c r="J39" t="n">
-        <v>1.11</v>
+        <v>1.15</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>21/10/2023 00:13</t>
+          <t>21/10/2023 00:43</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>1.25</v>
+        <v>1.19</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>22/10/2023 12:44</t>
+          <t>22/10/2023 12:45</t>
         </is>
       </c>
       <c r="N39" t="n">
-        <v>7</v>
+        <v>6.29</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>21/10/2023 00:13</t>
+          <t>21/10/2023 00:43</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>5.69</v>
+        <v>6.51</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>22/10/2023 12:51</t>
+          <t>22/10/2023 12:45</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>9.710000000000001</v>
+        <v>8.19</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>21/10/2023 00:13</t>
+          <t>21/10/2023 00:43</t>
         </is>
       </c>
       <c r="T39" t="n">
-        <v>7.79</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>22/10/2023 12:46</t>
+          <t>22/10/2023 12:45</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/cambodia/cpl/svay-rieng-kirivong-sok-sen-chey/vaoqpBvA/</t>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/visakha-angkor-tiger/8YkmqVgG/</t>
         </is>
       </c>
     </row>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>NagaWorld</t>
+          <t>Dangkor</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -4077,14 +4077,14 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Tiffy Army</t>
+          <t>Boeung Ket</t>
         </is>
       </c>
       <c r="I40" t="n">
         <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>1.84</v>
+        <v>4.37</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -4092,15 +4092,15 @@
         </is>
       </c>
       <c r="L40" t="n">
-        <v>1.95</v>
+        <v>4.18</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>22/10/2023 12:43</t>
+          <t>22/10/2023 12:44</t>
         </is>
       </c>
       <c r="N40" t="n">
-        <v>3.45</v>
+        <v>4.07</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -4108,15 +4108,15 @@
         </is>
       </c>
       <c r="P40" t="n">
-        <v>3.73</v>
+        <v>4.44</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>22/10/2023 12:43</t>
+          <t>22/10/2023 12:44</t>
         </is>
       </c>
       <c r="R40" t="n">
-        <v>3.27</v>
+        <v>1.48</v>
       </c>
       <c r="S40" t="inlineStr">
         <is>
@@ -4124,16 +4124,16 @@
         </is>
       </c>
       <c r="T40" t="n">
-        <v>3.07</v>
+        <v>1.56</v>
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>22/10/2023 12:43</t>
+          <t>22/10/2023 12:44</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/cambodia/cpl/nagaworld-tiffy-army/69VNxTWq/</t>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/dangkor-senchey-boeung-ket/nPlirk9M/</t>
         </is>
       </c>
     </row>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Dangkor</t>
+          <t>NagaWorld</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -4169,14 +4169,14 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Boeung Ket</t>
+          <t>Tiffy Army</t>
         </is>
       </c>
       <c r="I41" t="n">
         <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>4.37</v>
+        <v>1.84</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
@@ -4184,15 +4184,15 @@
         </is>
       </c>
       <c r="L41" t="n">
-        <v>4.18</v>
+        <v>1.95</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>22/10/2023 12:44</t>
+          <t>22/10/2023 12:43</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>4.07</v>
+        <v>3.45</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -4200,15 +4200,15 @@
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.44</v>
+        <v>3.73</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>22/10/2023 12:44</t>
+          <t>22/10/2023 12:43</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>1.48</v>
+        <v>3.27</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
@@ -4216,16 +4216,16 @@
         </is>
       </c>
       <c r="T41" t="n">
-        <v>1.56</v>
+        <v>3.07</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>22/10/2023 12:44</t>
+          <t>22/10/2023 12:43</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/cambodia/cpl/dangkor-senchey-boeung-ket/nPlirk9M/</t>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/nagaworld-tiffy-army/69VNxTWq/</t>
         </is>
       </c>
     </row>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>NagaWorld</t>
+          <t>Dangkor</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -5733,63 +5733,63 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Svay Rieng</t>
+          <t>Visakha</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>5.99</v>
+        <v>8.35</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>03/12/2023 00:42</t>
+          <t>03/12/2023 00:12</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>6.06</v>
+        <v>6.57</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>03/12/2023 10:05</t>
+          <t>03/12/2023 11:40</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>4.61</v>
+        <v>6.02</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>03/12/2023 00:42</t>
+          <t>03/12/2023 00:12</t>
         </is>
       </c>
       <c r="P58" t="n">
-        <v>4.65</v>
+        <v>5.34</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>03/12/2023 10:05</t>
+          <t>03/12/2023 11:40</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>1.37</v>
+        <v>1.2</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>03/12/2023 00:42</t>
+          <t>03/12/2023 00:12</t>
         </is>
       </c>
       <c r="T58" t="n">
-        <v>1.38</v>
+        <v>1.31</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>03/12/2023 10:05</t>
+          <t>03/12/2023 11:39</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/cambodia/cpl/nagaworld-svay-rieng/6mIYjJif/</t>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/dangkor-senchey-visakha/S26skcM6/</t>
         </is>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Dangkor</t>
+          <t>NagaWorld</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -5825,63 +5825,63 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Visakha</t>
+          <t>Svay Rieng</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>8.35</v>
+        <v>5.99</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>03/12/2023 00:12</t>
+          <t>03/12/2023 00:42</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>6.57</v>
+        <v>6.06</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>03/12/2023 11:40</t>
+          <t>03/12/2023 10:05</t>
         </is>
       </c>
       <c r="N59" t="n">
-        <v>6.02</v>
+        <v>4.61</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>03/12/2023 00:12</t>
+          <t>03/12/2023 00:42</t>
         </is>
       </c>
       <c r="P59" t="n">
-        <v>5.34</v>
+        <v>4.65</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>03/12/2023 11:40</t>
+          <t>03/12/2023 10:05</t>
         </is>
       </c>
       <c r="R59" t="n">
-        <v>1.2</v>
+        <v>1.37</v>
       </c>
       <c r="S59" t="inlineStr">
         <is>
-          <t>03/12/2023 00:12</t>
+          <t>03/12/2023 00:42</t>
         </is>
       </c>
       <c r="T59" t="n">
-        <v>1.31</v>
+        <v>1.38</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>03/12/2023 11:39</t>
+          <t>03/12/2023 10:05</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/cambodia/cpl/dangkor-senchey-visakha/S26skcM6/</t>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/nagaworld-svay-rieng/6mIYjJif/</t>
         </is>
       </c>
     </row>
@@ -7630,6 +7630,282 @@
       <c r="V78" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/cambodia/cpl/nagaworld-boeung-ket/G06gHF5a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>cambodia</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>cpl</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>45298.5</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Svay Rieng</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Prey Veng</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>07/01/2024 01:12</t>
+        </is>
+      </c>
+      <c r="L79" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:33</t>
+        </is>
+      </c>
+      <c r="N79" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>07/01/2024 01:12</t>
+        </is>
+      </c>
+      <c r="P79" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:56</t>
+        </is>
+      </c>
+      <c r="R79" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>07/01/2024 01:12</t>
+        </is>
+      </c>
+      <c r="T79" t="n">
+        <v>9.91</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:56</t>
+        </is>
+      </c>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/svay-rieng-prey-veng/z3MfFgzC/</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>cambodia</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>cpl</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>45298.5</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Phnom Penh Crown</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>3</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Angkor Tiger</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>2</v>
+      </c>
+      <c r="J80" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>07/01/2024 01:12</t>
+        </is>
+      </c>
+      <c r="L80" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:58</t>
+        </is>
+      </c>
+      <c r="N80" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>07/01/2024 01:12</t>
+        </is>
+      </c>
+      <c r="P80" t="n">
+        <v>7.33</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:59</t>
+        </is>
+      </c>
+      <c r="R80" t="n">
+        <v>9.52</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>07/01/2024 01:12</t>
+        </is>
+      </c>
+      <c r="T80" t="n">
+        <v>9.970000000000001</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:59</t>
+        </is>
+      </c>
+      <c r="V80" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/phnom-penh-crown-angkor-tiger/EgLbEDkI/</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>cambodia</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>cpl</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>45298.5</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Visakha</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Tiffy Army</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>2</v>
+      </c>
+      <c r="J81" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>07/01/2024 02:12</t>
+        </is>
+      </c>
+      <c r="L81" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:58</t>
+        </is>
+      </c>
+      <c r="N81" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>07/01/2024 02:12</t>
+        </is>
+      </c>
+      <c r="P81" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:58</t>
+        </is>
+      </c>
+      <c r="R81" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>07/01/2024 02:12</t>
+        </is>
+      </c>
+      <c r="T81" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>07/01/2024 11:58</t>
+        </is>
+      </c>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/cambodia/cpl/visakha-tiffy-army/fi5cGZK5/</t>
         </is>
       </c>
     </row>

</xml_diff>